<commit_message>
Weight and mean square error code added
</commit_message>
<xml_diff>
--- a/TDataEx.xlsx
+++ b/TDataEx.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADITYA\GithubDesktop\CP302\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D93B02A-FD8F-4D41-A911-0ADA66087D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB5662B-5FB5-4B58-AEC5-A148E706F97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
   <si>
     <t>S.No.</t>
   </si>
@@ -578,7 +578,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1247,7 +1247,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="5">
         <v>31.55</v>
@@ -1268,22 +1268,22 @@
         <v>72.150000000000006</v>
       </c>
       <c r="K14" s="5">
-        <v>1</v>
-      </c>
-      <c r="L14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="O14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P14" s="5">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -1291,34 +1291,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15" s="5">
-        <v>21.8</v>
+        <v>31.55</v>
       </c>
       <c r="F15" s="5">
-        <v>8.9600000000000009</v>
+        <v>16.22</v>
       </c>
       <c r="G15" s="5">
-        <v>15.38</v>
+        <v>23.88</v>
       </c>
       <c r="H15" s="5">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="I15" s="5">
-        <v>81.8</v>
+        <v>52.4</v>
       </c>
       <c r="J15" s="5">
-        <v>59.57</v>
+        <v>72.150000000000006</v>
       </c>
       <c r="K15" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>39</v>
@@ -1327,13 +1327,13 @@
         <v>35</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P15" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -1341,34 +1341,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C16" s="5">
         <v>34</v>
       </c>
       <c r="D16" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E16" s="5">
-        <v>31.96</v>
+        <v>21.8</v>
       </c>
       <c r="F16" s="5">
-        <v>21.85</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="G16" s="5">
-        <v>26.91</v>
+        <v>15.38</v>
       </c>
       <c r="H16" s="5">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I16" s="5">
-        <v>192</v>
+        <v>81.8</v>
       </c>
       <c r="J16" s="5">
-        <v>79.180000000000007</v>
+        <v>59.57</v>
       </c>
       <c r="K16" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>39</v>
@@ -1377,13 +1377,13 @@
         <v>35</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P16" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
@@ -1391,34 +1391,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5">
         <v>3</v>
       </c>
       <c r="E17" s="5">
-        <v>34.26</v>
+        <v>31.96</v>
       </c>
       <c r="F17" s="5">
-        <v>23.38</v>
+        <v>21.85</v>
       </c>
       <c r="G17" s="5">
-        <v>28.82</v>
+        <v>26.91</v>
       </c>
       <c r="H17" s="5">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I17" s="5">
-        <v>250</v>
+        <v>192</v>
       </c>
       <c r="J17" s="5">
-        <v>81.42</v>
+        <v>79.180000000000007</v>
       </c>
       <c r="K17" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>39</v>
@@ -1427,13 +1427,13 @@
         <v>35</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="O17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="P17" s="5">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -1441,55 +1441,100 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D18" s="5">
         <v>3</v>
       </c>
       <c r="E18" s="5">
-        <v>35.5</v>
+        <v>34.26</v>
       </c>
       <c r="F18" s="5">
-        <v>20.2</v>
+        <v>23.38</v>
       </c>
       <c r="G18" s="5">
-        <v>27.8</v>
+        <v>28.82</v>
       </c>
       <c r="H18" s="5">
-        <v>50.9</v>
+        <v>83</v>
       </c>
       <c r="I18" s="5">
-        <v>6.4</v>
+        <v>250</v>
       </c>
       <c r="J18" s="5">
-        <v>75.3</v>
+        <v>81.42</v>
       </c>
       <c r="K18" s="5">
         <v>1</v>
       </c>
       <c r="L18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5">
+        <v>33</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>35.5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="G19" s="5">
+        <v>27.8</v>
+      </c>
+      <c r="H19" s="5">
+        <v>50.9</v>
+      </c>
+      <c r="I19" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="J19" s="5">
+        <v>75.3</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="O19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>

</xml_diff>